<commit_message>
ENH: Add asmp_id and mp_file_id
</commit_message>
<xml_diff>
--- a/lifelib/libraries/appliedlife/model_parameters.xlsx
+++ b/lifelib/libraries/appliedlife/model_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\lifelib\lifelib\libraries\appliedlife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1379F6B-4953-4CA1-9F87-DD1C925E1CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEA0138-0F20-42E7-9E21-1C18E38A794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{AFC81F58-63C7-4FF4-94D0-E1EA68308CE5}"/>
   </bookViews>
@@ -18,8 +18,6 @@
     <sheet name="RunParams" sheetId="1" r:id="rId3"/>
     <sheet name="SpaceParams" sheetId="2" r:id="rId4"/>
     <sheet name="GMXB" sheetId="5" r:id="rId5"/>
-    <sheet name="GLWB" sheetId="6" r:id="rId6"/>
-    <sheet name="VUL" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ParamList!$A$1:$C$15</definedName>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
   <si>
     <t>run_id</t>
   </si>
@@ -80,12 +78,6 @@
     <t>Model point file location</t>
   </si>
   <si>
-    <t>asmp_file</t>
-  </si>
-  <si>
-    <t>Assumption file name</t>
-  </si>
-  <si>
     <t>read_from</t>
   </si>
   <si>
@@ -98,9 +90,6 @@
     <t>product_id</t>
   </si>
   <si>
-    <t>scen_file</t>
-  </si>
-  <si>
     <t>Economic scenaio file name</t>
   </si>
   <si>
@@ -116,84 +105,33 @@
     <t>GMAB</t>
   </si>
   <si>
-    <t>GMWB</t>
-  </si>
-  <si>
     <t>Base run end of Dec 2022</t>
   </si>
   <si>
-    <t>scenaio_202312.xlsx</t>
-  </si>
-  <si>
-    <t>scenaio_202212.xlsx</t>
-  </si>
-  <si>
-    <t>disc_file</t>
-  </si>
-  <si>
     <t>Discount Rate file</t>
   </si>
   <si>
-    <t>discount_rates_20221231.xlsx</t>
-  </si>
-  <si>
-    <t>discount_rates_20231231.xlsx</t>
-  </si>
-  <si>
-    <t>sensitivity</t>
-  </si>
-  <si>
     <t>GMDB</t>
   </si>
   <si>
     <t>has_gmdb</t>
   </si>
   <si>
-    <t>wdraw_rate</t>
-  </si>
-  <si>
     <t>is_prem_guar</t>
   </si>
   <si>
-    <t>has_adb</t>
-  </si>
-  <si>
-    <t>assumptions_2023.xlsx</t>
-  </si>
-  <si>
-    <t>assumptions_2022.xlsx</t>
-  </si>
-  <si>
     <t>maint_fee_rate</t>
   </si>
   <si>
-    <t>PLAN01</t>
-  </si>
-  <si>
-    <t>PLAN02</t>
-  </si>
-  <si>
     <t>mort_file</t>
   </si>
   <si>
     <t>mortality_tables.xlsx</t>
   </si>
   <si>
-    <t>Life_S</t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
-    <t>segment_id</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>model_point_file_stem</t>
-  </si>
-  <si>
     <t>202312</t>
   </si>
   <si>
@@ -203,12 +141,6 @@
     <t>model_point</t>
   </si>
   <si>
-    <t>VUL</t>
-  </si>
-  <si>
-    <t>adb_ratio</t>
-  </si>
-  <si>
     <t>model_point_data</t>
   </si>
   <si>
@@ -311,27 +243,15 @@
     <t>asmp_id</t>
   </si>
   <si>
-    <t>202312_INTUP</t>
-  </si>
-  <si>
     <t>BASE</t>
   </si>
   <si>
-    <t>MORT_UP</t>
-  </si>
-  <si>
-    <t>INT_UP</t>
-  </si>
-  <si>
     <t>economic_data</t>
   </si>
   <si>
     <t>risk_free</t>
   </si>
   <si>
-    <t>int_rate_prefix</t>
-  </si>
-  <si>
     <t>scen_param_file</t>
   </si>
   <si>
@@ -401,13 +321,37 @@
     <t>is_lapse_dynamic</t>
   </si>
   <si>
-    <t>Sensitivity ID in string</t>
-  </si>
-  <si>
     <t>Interest rate sensitivity ID in string</t>
   </si>
   <si>
     <t>Wheter the lapse assumption is dynamic in boolean</t>
+  </si>
+  <si>
+    <t>FIA</t>
+  </si>
+  <si>
+    <t>model_point_file_prefix</t>
+  </si>
+  <si>
+    <t>scen_file_prefix</t>
+  </si>
+  <si>
+    <t>202401NB</t>
+  </si>
+  <si>
+    <t>mp_file_id</t>
+  </si>
+  <si>
+    <t>2023Q4IF</t>
+  </si>
+  <si>
+    <t>2022Q4IF</t>
+  </si>
+  <si>
+    <t>Assumption file ID</t>
+  </si>
+  <si>
+    <t>Model point file ID</t>
   </si>
 </sst>
 </file>
@@ -786,7 +730,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -798,10 +742,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -809,13 +753,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +767,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -831,21 +775,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -853,160 +797,161 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C15" xr:uid="{87613B9D-8C88-4F99-8DFC-DD6EA5034DE4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48D33D2-B2B8-43CE-86B3-3DE4241614D4}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1018,7 +963,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -1026,71 +971,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1101,215 +1041,158 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDE9C88-B23F-452D-8C16-20C46E0FE76B}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.07421875" customWidth="1"/>
-    <col min="3" max="3" width="19.4609375" customWidth="1"/>
-    <col min="4" max="4" width="21.53515625" customWidth="1"/>
-    <col min="5" max="5" width="26.84375" customWidth="1"/>
-    <col min="6" max="6" width="14.53515625" customWidth="1"/>
-    <col min="7" max="7" width="14.61328125" customWidth="1"/>
-    <col min="8" max="8" width="11.921875" customWidth="1"/>
-    <col min="9" max="9" width="13.84375" customWidth="1"/>
-    <col min="10" max="10" width="37.765625" customWidth="1"/>
+    <col min="3" max="3" width="11.921875" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" customWidth="1"/>
+    <col min="5" max="5" width="11.765625" customWidth="1"/>
+    <col min="6" max="6" width="14.61328125" customWidth="1"/>
+    <col min="7" max="7" width="37.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>45291</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>45291</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>45291</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>45291</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>44926</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1323,7 +1206,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1337,24 +1220,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>5000</v>
@@ -1363,7 +1246,7 @@
         <v>500</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1371,7 +1254,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>5000</v>
@@ -1380,7 +1263,7 @@
         <v>500</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1388,7 +1271,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>6000</v>
@@ -1397,7 +1280,7 @@
         <v>600</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1414,7 +1297,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1438,63 +1321,63 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O1" t="s">
-        <v>84</v>
-      </c>
       <c r="P1" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="Q1" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1503,13 +1386,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="H2">
         <v>0.1</v>
@@ -1524,19 +1407,19 @@
         <v>0.03</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="O2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="P2" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="Q2" s="2">
         <v>0</v>
@@ -1544,10 +1427,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1556,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1574,19 +1457,19 @@
         <v>0.03</v>
       </c>
       <c r="L3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" t="s">
         <v>79</v>
       </c>
-      <c r="M3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3" t="s">
-        <v>105</v>
-      </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="P3" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="Q3" s="2">
         <v>0</v>
@@ -1594,10 +1477,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -1606,13 +1489,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="H4">
         <v>0.1</v>
@@ -1627,19 +1510,19 @@
         <v>0.05</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="O4" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="P4" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="Q4" s="2">
         <v>0.03</v>
@@ -1647,10 +1530,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -1659,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1677,187 +1560,22 @@
         <v>0.05</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="M5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" t="s">
         <v>80</v>
       </c>
-      <c r="N5" t="s">
-        <v>106</v>
-      </c>
       <c r="O5" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="P5" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="Q5" s="2">
         <v>0.05</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DACB1A-90CC-4A24-A35E-89551E8B413D}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.84375" customWidth="1"/>
-    <col min="2" max="2" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.07421875" customWidth="1"/>
-    <col min="4" max="4" width="17.23046875" customWidth="1"/>
-    <col min="5" max="5" width="15.15234375" customWidth="1"/>
-    <col min="6" max="6" width="14.61328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.06</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46087B2F-8C48-4C3E-B65C-6FE8CEEBCC67}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="14.07421875" customWidth="1"/>
-    <col min="5" max="5" width="10.23046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Add mortality scalar
</commit_message>
<xml_diff>
--- a/lifelib/libraries/appliedlife/model_parameters.xlsx
+++ b/lifelib/libraries/appliedlife/model_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e058ec69bd94c7d/pyproj/lifelib/lifelib/libraries/appliedlife/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\lifelib\lifelib\libraries\appliedlife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2EABB00B-F338-4CF3-A194-16F4ADFA045E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8F2090E-BC1D-4906-8B25-C823B53C94D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CB4875-DF52-4D14-865D-B729F158A39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{AFC81F58-63C7-4FF4-94D0-E1EA68308CE5}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{AFC81F58-63C7-4FF4-94D0-E1EA68308CE5}"/>
   </bookViews>
   <sheets>
     <sheet name="ParamList" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>run_id</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>has_gmab</t>
+  </si>
+  <si>
+    <t>mort_scalar_id</t>
+  </si>
+  <si>
+    <t>M001</t>
   </si>
 </sst>
 </file>
@@ -951,7 +957,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1043,8 +1049,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1294,10 +1300,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D39E09-302B-4AC1-86FE-96F3B3810039}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1314,12 +1320,12 @@
     <col min="10" max="10" width="15.15234375" customWidth="1"/>
     <col min="11" max="11" width="15.921875" customWidth="1"/>
     <col min="12" max="12" width="14.921875" customWidth="1"/>
-    <col min="13" max="13" width="16.61328125" customWidth="1"/>
-    <col min="14" max="14" width="12.23046875" customWidth="1"/>
-    <col min="15" max="15" width="12.07421875" customWidth="1"/>
+    <col min="13" max="14" width="16.61328125" customWidth="1"/>
+    <col min="15" max="15" width="12.23046875" customWidth="1"/>
+    <col min="16" max="16" width="12.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1360,19 +1366,22 @@
         <v>54</v>
       </c>
       <c r="N1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" t="s">
         <v>57</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>60</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1413,19 +1422,22 @@
         <v>56</v>
       </c>
       <c r="N2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>61</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1463,19 +1475,22 @@
         <v>56</v>
       </c>
       <c r="N3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" t="s">
         <v>77</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>61</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1516,19 +1531,22 @@
         <v>56</v>
       </c>
       <c r="N4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4" t="s">
         <v>59</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>62</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1566,15 +1584,18 @@
         <v>56</v>
       </c>
       <c r="N5" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" t="s">
         <v>78</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>62</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>0.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: Parameterize assumption file prefix
</commit_message>
<xml_diff>
--- a/lifelib/libraries/appliedlife/model_parameters.xlsx
+++ b/lifelib/libraries/appliedlife/model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\lifelib\lifelib\libraries\appliedlife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CB4875-DF52-4D14-865D-B729F158A39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF63BFD9-A935-4F60-890B-A540727988AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{AFC81F58-63C7-4FF4-94D0-E1EA68308CE5}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{AFC81F58-63C7-4FF4-94D0-E1EA68308CE5}"/>
   </bookViews>
   <sheets>
     <sheet name="ParamList" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="GMXB" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ParamList!$A$1:$C$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ParamList!$A$1:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
   <si>
     <t>run_id</t>
   </si>
@@ -324,9 +324,6 @@
     <t>FIA</t>
   </si>
   <si>
-    <t>model_point_file_prefix</t>
-  </si>
-  <si>
     <t>scen_file_prefix</t>
   </si>
   <si>
@@ -358,6 +355,18 @@
   </si>
   <si>
     <t>M001</t>
+  </si>
+  <si>
+    <t>asmp_file_prefix</t>
+  </si>
+  <si>
+    <t>assumptions</t>
+  </si>
+  <si>
+    <t>Stem part of the assumption file name</t>
+  </si>
+  <si>
+    <t>mp_file_prefix</t>
   </si>
 </sst>
 </file>
@@ -733,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87613B9D-8C88-4F99-8DFC-DD6EA5034DE4}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -781,7 +790,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -792,95 +801,95 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -891,61 +900,72 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>89</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C15" xr:uid="{87613B9D-8C88-4F99-8DFC-DD6EA5034DE4}"/>
+  <autoFilter ref="A1:C16" xr:uid="{87613B9D-8C88-4F99-8DFC-DD6EA5034DE4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -954,10 +974,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48D33D2-B2B8-43CE-86B3-3DE4241614D4}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -985,7 +1005,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -993,49 +1013,57 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1049,8 +1077,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1102,7 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>63</v>
@@ -1097,7 +1125,7 @@
         <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>27</v>
@@ -1106,7 +1134,7 @@
         <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1120,7 +1148,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>27</v>
@@ -1143,7 +1171,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>27</v>
@@ -1166,7 +1194,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>27</v>
@@ -1189,7 +1217,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>28</v>
@@ -1303,7 +1331,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1364,7 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
         <v>34</v>
@@ -1366,7 +1394,7 @@
         <v>54</v>
       </c>
       <c r="N1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O1" t="s">
         <v>57</v>
@@ -1422,7 +1450,7 @@
         <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O2" t="s">
         <v>58</v>
@@ -1475,7 +1503,7 @@
         <v>56</v>
       </c>
       <c r="N3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O3" t="s">
         <v>77</v>
@@ -1531,7 +1559,7 @@
         <v>56</v>
       </c>
       <c r="N4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O4" t="s">
         <v>59</v>
@@ -1584,7 +1612,7 @@
         <v>56</v>
       </c>
       <c r="N5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O5" t="s">
         <v>78</v>

</xml_diff>